<commit_message>
refactoring results modules so that `Activity_ID` matches activities modules
</commit_message>
<xml_diff>
--- a/data/bob/2021_prwi_sites_bob.xlsx
+++ b/data/bob/2021_prwi_sites_bob.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwainright\OneDrive - DOI\Documents\data_projects\2023\iss156_bss_edd\data\bob\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497BF68F-4CFF-442F-8249-D4F0B2A83E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF70B020-805A-4A73-A0CE-FB72648AE26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{270734E7-F507-4A64-894A-D3055E06BC53}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="2" xr2:uid="{270734E7-F507-4A64-894A-D3055E06BC53}"/>
   </bookViews>
   <sheets>
     <sheet name="water chem" sheetId="1" r:id="rId1"/>
@@ -1052,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC88A5C9-0B74-4ABC-9BC6-F2FC87F31767}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1835,8 +1835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089A971F-D988-401A-9F07-71E8D5320105}">
   <dimension ref="A1:D179"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2422,8 +2422,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="20" t="s">
-        <v>37</v>
+      <c r="A42" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>53</v>
@@ -2436,8 +2436,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="20" t="s">
-        <v>37</v>
+      <c r="A43" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B43" s="20" t="s">
         <v>97</v>
@@ -2450,8 +2450,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="20" t="s">
-        <v>37</v>
+      <c r="A44" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B44" s="20" t="s">
         <v>55</v>
@@ -2464,8 +2464,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="20" t="s">
-        <v>37</v>
+      <c r="A45" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B45" s="20" t="s">
         <v>113</v>
@@ -2478,8 +2478,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="20" t="s">
-        <v>37</v>
+      <c r="A46" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B46" s="20" t="s">
         <v>115</v>
@@ -2492,8 +2492,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="20" t="s">
-        <v>37</v>
+      <c r="A47" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B47" s="20" t="s">
         <v>117</v>
@@ -2506,8 +2506,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="20" t="s">
-        <v>37</v>
+      <c r="A48" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>63</v>
@@ -2520,8 +2520,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="20" t="s">
-        <v>37</v>
+      <c r="A49" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>65</v>
@@ -2534,8 +2534,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="20" t="s">
-        <v>37</v>
+      <c r="A50" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B50" s="20" t="s">
         <v>69</v>
@@ -2548,8 +2548,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="20" t="s">
-        <v>37</v>
+      <c r="A51" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>119</v>
@@ -2562,8 +2562,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="20" t="s">
-        <v>37</v>
+      <c r="A52" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>121</v>
@@ -2576,8 +2576,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="20" t="s">
-        <v>37</v>
+      <c r="A53" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B53" s="20" t="s">
         <v>79</v>
@@ -2590,8 +2590,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="20" t="s">
-        <v>37</v>
+      <c r="A54" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>81</v>
@@ -2604,8 +2604,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="20" t="s">
-        <v>37</v>
+      <c r="A55" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>123</v>
@@ -2618,8 +2618,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="20" t="s">
-        <v>37</v>
+      <c r="A56" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B56" s="20" t="s">
         <v>125</v>
@@ -2632,8 +2632,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="20" t="s">
-        <v>37</v>
+      <c r="A57" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B57" s="20" t="s">
         <v>87</v>
@@ -2646,8 +2646,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="20" t="s">
-        <v>37</v>
+      <c r="A58" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>127</v>
@@ -2660,8 +2660,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="20" t="s">
-        <v>37</v>
+      <c r="A59" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B59" s="20" t="s">
         <v>129</v>
@@ -2674,8 +2674,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="20" t="s">
-        <v>37</v>
+      <c r="A60" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B60" s="20" t="s">
         <v>89</v>
@@ -2688,8 +2688,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="20" t="s">
-        <v>37</v>
+      <c r="A61" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B61" s="20" t="s">
         <v>91</v>
@@ -2702,8 +2702,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A62" s="22" t="s">
-        <v>37</v>
+      <c r="A62" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B62" s="22" t="s">
         <v>109</v>
@@ -4359,6 +4359,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CDF426C5941C634898DECC69F43B1B84" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ddb6186b385e9e586dbf2c2d396412c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a26c063d-e4ab-4c2c-a5f9-3b05989843c6" xmlns:ns3="31062a0d-ede8-4112-b4bb-00a9c1bc8e16" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41634503152380488122de28a01d3282" ns2:_="" ns3:_="">
     <xsd:import namespace="a26c063d-e4ab-4c2c-a5f9-3b05989843c6"/>
@@ -4553,16 +4562,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2C79F29-776A-478F-AC44-3E61F39C5C2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F6C018F-5658-4AB1-87EA-C991B973A7AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4579,12 +4587,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2C79F29-776A-478F-AC44-3E61F39C5C2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added code to correct for missing and erroneous values in source spreadsheet
</commit_message>
<xml_diff>
--- a/data/bob/2021_prwi_sites_bob.xlsx
+++ b/data/bob/2021_prwi_sites_bob.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwainright\OneDrive - DOI\Documents\data_projects\2023\iss156_bss_edd\data\bob\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/dgjones_nps_gov/Documents/01-NPS/IMD/NCRN/MONITORING/MBSS/08_DATA/2021/Deliverables from UMCES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF70B020-805A-4A73-A0CE-FB72648AE26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{1CB9A33A-6348-4342-B7B8-6230238209EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D12C5587-9AEE-4130-B631-8181E5AA4AA7}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="2" xr2:uid="{270734E7-F507-4A64-894A-D3055E06BC53}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{270734E7-F507-4A64-894A-D3055E06BC53}"/>
   </bookViews>
   <sheets>
     <sheet name="water chem" sheetId="1" r:id="rId1"/>
@@ -575,7 +575,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1052,24 +1052,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC88A5C9-0B74-4ABC-9BC6-F2FC87F31767}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.68359375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="49.5" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:9" ht="51.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>1.4219999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>1.355</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>1.9059999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>1.9179999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>1.9650000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>1.5569999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>1.5820000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>9.0220000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
@@ -1431,17 +1431,17 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.578125" customWidth="1"/>
-    <col min="3" max="3" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.578125" customWidth="1"/>
-    <col min="7" max="7" width="11.83984375" customWidth="1"/>
-    <col min="9" max="9" width="18.68359375" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="45.75" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10">
       <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10">
       <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10">
       <c r="A4" s="15" t="s">
         <v>37</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10">
       <c r="A5" s="15" t="s">
         <v>14</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10">
       <c r="A6" s="15" t="s">
         <v>17</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10">
       <c r="A7" s="15" t="s">
         <v>18</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10">
       <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10">
       <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1">
       <c r="A10" s="17" t="s">
         <v>21</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10">
       <c r="B14" t="s">
         <v>45</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10">
       <c r="A15" s="15" t="s">
         <v>9</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10">
       <c r="A16" s="15" t="s">
         <v>9</v>
       </c>
@@ -1791,37 +1791,37 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1">
       <c r="A17" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:1">
       <c r="A18" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:1">
       <c r="A19" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:1">
       <c r="A20" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:1">
       <c r="A21" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:1">
       <c r="A22" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:1">
       <c r="A23" s="15" t="s">
         <v>9</v>
       </c>
@@ -1835,19 +1835,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089A971F-D988-401A-9F07-71E8D5320105}">
   <dimension ref="A1:D179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1">
       <c r="A1" s="19" t="s">
         <v>47</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="20" t="s">
         <v>9</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="20" t="s">
         <v>9</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="20" t="s">
         <v>9</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="20" t="s">
         <v>9</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="20" t="s">
         <v>9</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" ht="15.75">
       <c r="A8" s="20" t="s">
         <v>9</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" ht="15.75">
       <c r="A9" s="20" t="s">
         <v>9</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" ht="15.75">
       <c r="A10" s="20" t="s">
         <v>9</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" ht="15.75">
       <c r="A11" s="20" t="s">
         <v>9</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" ht="15.75">
       <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" ht="15.75">
       <c r="A13" s="20" t="s">
         <v>9</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="20" t="s">
         <v>9</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" ht="15.75">
       <c r="A15" s="20" t="s">
         <v>9</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" ht="15.75">
       <c r="A16" s="20" t="s">
         <v>9</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" ht="15.75">
       <c r="A17" s="20" t="s">
         <v>9</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" ht="15.75">
       <c r="A18" s="20" t="s">
         <v>9</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" ht="15.75">
       <c r="A19" s="20" t="s">
         <v>9</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" ht="15.75">
       <c r="A20" s="20" t="s">
         <v>9</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="20" t="s">
         <v>9</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" ht="15.75">
       <c r="A22" s="20" t="s">
         <v>9</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" ht="15.75">
       <c r="A23" s="20" t="s">
         <v>9</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:4" ht="16.5" thickBot="1">
       <c r="A24" s="22" t="s">
         <v>9</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" ht="15.75">
       <c r="A25" s="20" t="s">
         <v>11</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" ht="15.75">
       <c r="A26" s="20" t="s">
         <v>11</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:4" ht="15.75">
       <c r="A27" s="20" t="s">
         <v>11</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:4" ht="15.75">
       <c r="A28" s="20" t="s">
         <v>11</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:4" ht="15.75">
       <c r="A29" s="20" t="s">
         <v>11</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:4" ht="15.75">
       <c r="A30" s="20" t="s">
         <v>11</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:4" ht="15.75">
       <c r="A31" s="20" t="s">
         <v>11</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:4" ht="15.75">
       <c r="A32" s="20" t="s">
         <v>11</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" ht="15.75">
       <c r="A33" s="20" t="s">
         <v>11</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" ht="15.75">
       <c r="A34" s="20" t="s">
         <v>11</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:4" ht="15.75">
       <c r="A35" s="20" t="s">
         <v>11</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:4" ht="15.75">
       <c r="A36" s="20" t="s">
         <v>11</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:4" ht="15.75">
       <c r="A37" s="20" t="s">
         <v>11</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" ht="15.75">
       <c r="A38" s="20" t="s">
         <v>11</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" ht="15.75">
       <c r="A39" s="20" t="s">
         <v>11</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:4" ht="15.75">
       <c r="A40" s="20" t="s">
         <v>11</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="41" spans="1:4" ht="16.5" thickBot="1">
       <c r="A41" s="22" t="s">
         <v>11</v>
       </c>
@@ -2421,9 +2421,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="2" t="s">
-        <v>12</v>
+    <row r="42" spans="1:4" ht="15.75">
+      <c r="A42" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>53</v>
@@ -2435,9 +2435,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="2" t="s">
-        <v>12</v>
+    <row r="43" spans="1:4" ht="15.75">
+      <c r="A43" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B43" s="20" t="s">
         <v>97</v>
@@ -2449,9 +2449,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="2" t="s">
-        <v>12</v>
+    <row r="44" spans="1:4" ht="15.75">
+      <c r="A44" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B44" s="20" t="s">
         <v>55</v>
@@ -2463,9 +2463,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="2" t="s">
-        <v>12</v>
+    <row r="45" spans="1:4" ht="15.75">
+      <c r="A45" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B45" s="20" t="s">
         <v>113</v>
@@ -2477,9 +2477,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="2" t="s">
-        <v>12</v>
+    <row r="46" spans="1:4" ht="15.75">
+      <c r="A46" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B46" s="20" t="s">
         <v>115</v>
@@ -2491,9 +2491,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="2" t="s">
-        <v>12</v>
+    <row r="47" spans="1:4" ht="15.75">
+      <c r="A47" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B47" s="20" t="s">
         <v>117</v>
@@ -2505,9 +2505,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="2" t="s">
-        <v>12</v>
+    <row r="48" spans="1:4" ht="15.75">
+      <c r="A48" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>63</v>
@@ -2519,9 +2519,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="2" t="s">
-        <v>12</v>
+    <row r="49" spans="1:4" ht="15.75">
+      <c r="A49" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>65</v>
@@ -2533,9 +2533,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="2" t="s">
-        <v>12</v>
+    <row r="50" spans="1:4" ht="15.75">
+      <c r="A50" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B50" s="20" t="s">
         <v>69</v>
@@ -2547,9 +2547,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="2" t="s">
-        <v>12</v>
+    <row r="51" spans="1:4" ht="15.75">
+      <c r="A51" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>119</v>
@@ -2561,9 +2561,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="2" t="s">
-        <v>12</v>
+    <row r="52" spans="1:4" ht="15.75">
+      <c r="A52" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>121</v>
@@ -2575,9 +2575,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="2" t="s">
-        <v>12</v>
+    <row r="53" spans="1:4" ht="15.75">
+      <c r="A53" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B53" s="20" t="s">
         <v>79</v>
@@ -2589,9 +2589,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="2" t="s">
-        <v>12</v>
+    <row r="54" spans="1:4" ht="15.75">
+      <c r="A54" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>81</v>
@@ -2603,9 +2603,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="2" t="s">
-        <v>12</v>
+    <row r="55" spans="1:4" ht="15.75">
+      <c r="A55" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>123</v>
@@ -2617,9 +2617,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="2" t="s">
-        <v>12</v>
+    <row r="56" spans="1:4" ht="15.75">
+      <c r="A56" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B56" s="20" t="s">
         <v>125</v>
@@ -2631,9 +2631,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="2" t="s">
-        <v>12</v>
+    <row r="57" spans="1:4" ht="15.75">
+      <c r="A57" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B57" s="20" t="s">
         <v>87</v>
@@ -2645,9 +2645,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="2" t="s">
-        <v>12</v>
+    <row r="58" spans="1:4" ht="15.75">
+      <c r="A58" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>127</v>
@@ -2659,9 +2659,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="2" t="s">
-        <v>12</v>
+    <row r="59" spans="1:4" ht="15.75">
+      <c r="A59" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B59" s="20" t="s">
         <v>129</v>
@@ -2673,9 +2673,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="2" t="s">
-        <v>12</v>
+    <row r="60" spans="1:4" ht="15.75">
+      <c r="A60" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B60" s="20" t="s">
         <v>89</v>
@@ -2687,9 +2687,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="2" t="s">
-        <v>12</v>
+    <row r="61" spans="1:4" ht="15.75">
+      <c r="A61" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B61" s="20" t="s">
         <v>91</v>
@@ -2701,9 +2701,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A62" s="2" t="s">
-        <v>12</v>
+    <row r="62" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A62" s="22" t="s">
+        <v>37</v>
       </c>
       <c r="B62" s="22" t="s">
         <v>109</v>
@@ -2715,7 +2715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:4" ht="15.75">
       <c r="A63" s="20" t="s">
         <v>14</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:4" ht="15.75">
       <c r="A64" s="20" t="s">
         <v>14</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:4" ht="15.75">
       <c r="A65" s="20" t="s">
         <v>14</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:4" ht="15.75">
       <c r="A66" s="20" t="s">
         <v>14</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:4" ht="15.75">
       <c r="A67" s="20" t="s">
         <v>14</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:4" ht="15.75">
       <c r="A68" s="20" t="s">
         <v>14</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:4" ht="15.75">
       <c r="A69" s="20" t="s">
         <v>14</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:4" ht="15.75">
       <c r="A70" s="20" t="s">
         <v>14</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:4" ht="15.75">
       <c r="A71" s="20" t="s">
         <v>14</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:4" ht="15.75">
       <c r="A72" s="20" t="s">
         <v>14</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:4" ht="15.75">
       <c r="A73" s="20" t="s">
         <v>14</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:4" ht="15.75">
       <c r="A74" s="20" t="s">
         <v>14</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:4" ht="15.75">
       <c r="A75" s="20" t="s">
         <v>14</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:4" ht="15.75">
       <c r="A76" s="20" t="s">
         <v>14</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:4" ht="15.75">
       <c r="A77" s="20" t="s">
         <v>14</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:4" ht="15.75">
       <c r="A78" s="20" t="s">
         <v>14</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:4" ht="15.75">
       <c r="A79" s="20" t="s">
         <v>14</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:4" ht="15.75">
       <c r="A80" s="20" t="s">
         <v>14</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:4" ht="15.75">
       <c r="A81" s="20" t="s">
         <v>14</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:4" ht="15.75">
       <c r="A82" s="20" t="s">
         <v>14</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="83" spans="1:4" ht="16.5" thickBot="1">
       <c r="A83" s="22" t="s">
         <v>14</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:4" ht="15.75">
       <c r="A84" s="20" t="s">
         <v>17</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:4" ht="15.75">
       <c r="A85" s="20" t="s">
         <v>17</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:4" ht="15.75">
       <c r="A86" s="20" t="s">
         <v>17</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:4" ht="15.75">
       <c r="A87" s="20" t="s">
         <v>17</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:4" ht="15.75">
       <c r="A88" s="20" t="s">
         <v>17</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:4" ht="15.75">
       <c r="A89" s="20" t="s">
         <v>17</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:4" ht="15.75">
       <c r="A90" s="20" t="s">
         <v>17</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:4" ht="15.75">
       <c r="A91" s="20" t="s">
         <v>17</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:4" ht="15.75">
       <c r="A92" s="20" t="s">
         <v>17</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:4" ht="15.75">
       <c r="A93" s="20" t="s">
         <v>17</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:4" ht="15.75">
       <c r="A94" s="20" t="s">
         <v>17</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:4" ht="15.75">
       <c r="A95" s="20" t="s">
         <v>17</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:4" ht="15.75">
       <c r="A96" s="20" t="s">
         <v>17</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:4" ht="15.75">
       <c r="A97" s="20" t="s">
         <v>17</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:4" ht="15.75">
       <c r="A98" s="20" t="s">
         <v>17</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="99" spans="1:4" ht="16.5" thickBot="1">
       <c r="A99" s="22" t="s">
         <v>17</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:4" ht="15.75">
       <c r="A100" s="20" t="s">
         <v>18</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:4" ht="15.75">
       <c r="A101" s="20" t="s">
         <v>18</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:4" ht="15.75">
       <c r="A102" s="20" t="s">
         <v>18</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:4" ht="15.75">
       <c r="A103" s="20" t="s">
         <v>18</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:4" ht="15.75">
       <c r="A104" s="20" t="s">
         <v>18</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:4" ht="15.75">
       <c r="A105" s="20" t="s">
         <v>18</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:4" ht="15.75">
       <c r="A106" s="20" t="s">
         <v>18</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:4" ht="15.75">
       <c r="A107" s="20" t="s">
         <v>18</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:4" ht="15.75">
       <c r="A108" s="20" t="s">
         <v>18</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:4" ht="15.75">
       <c r="A109" s="20" t="s">
         <v>18</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:4" ht="15.75">
       <c r="A110" s="20" t="s">
         <v>18</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:4" ht="15.75">
       <c r="A111" s="20" t="s">
         <v>18</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:4" ht="15.75">
       <c r="A112" s="20" t="s">
         <v>18</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:4" ht="15.75">
       <c r="A113" s="20" t="s">
         <v>18</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:4" ht="15.75">
       <c r="A114" s="20" t="s">
         <v>18</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="115" spans="1:4" ht="16.5" thickBot="1">
       <c r="A115" s="22" t="s">
         <v>18</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:4" ht="15.75">
       <c r="A116" s="20" t="s">
         <v>19</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:4" ht="15.75">
       <c r="A117" s="20" t="s">
         <v>19</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:4" ht="15.75">
       <c r="A118" s="20" t="s">
         <v>19</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:4" ht="15.75">
       <c r="A119" s="20" t="s">
         <v>19</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:4" ht="15.75">
       <c r="A120" s="20" t="s">
         <v>19</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:4" ht="15.75">
       <c r="A121" s="20" t="s">
         <v>19</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:4" ht="15.75">
       <c r="A122" s="20" t="s">
         <v>19</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:4" ht="15.75">
       <c r="A123" s="20" t="s">
         <v>19</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:4" ht="15.75">
       <c r="A124" s="20" t="s">
         <v>19</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:4" ht="15.75">
       <c r="A125" s="20" t="s">
         <v>19</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:4" ht="15.75">
       <c r="A126" s="20" t="s">
         <v>19</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:4" ht="15.75">
       <c r="A127" s="20" t="s">
         <v>19</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:4" ht="15.75">
       <c r="A128" s="20" t="s">
         <v>19</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:4" ht="15.75">
       <c r="A129" s="20" t="s">
         <v>19</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:4" ht="15.75">
       <c r="A130" s="20" t="s">
         <v>19</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:4" ht="15.75">
       <c r="A131" s="20" t="s">
         <v>19</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:4" ht="15.75">
       <c r="A132" s="20" t="s">
         <v>19</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:4" ht="15.75">
       <c r="A133" s="20" t="s">
         <v>19</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:4" ht="15.75">
       <c r="A134" s="20" t="s">
         <v>19</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:4" ht="15.75">
       <c r="A135" s="20" t="s">
         <v>19</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="136" spans="1:4" ht="16.5" thickBot="1">
       <c r="A136" s="22" t="s">
         <v>19</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:4" ht="15.75">
       <c r="A137" s="20" t="s">
         <v>20</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:4" ht="15.75">
       <c r="A138" s="20" t="s">
         <v>20</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:4" ht="15.75">
       <c r="A139" s="20" t="s">
         <v>20</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:4" ht="15.75">
       <c r="A140" s="20" t="s">
         <v>20</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:4" ht="15.75">
       <c r="A141" s="20" t="s">
         <v>20</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:4" ht="15.75">
       <c r="A142" s="20" t="s">
         <v>20</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:4" ht="15.75">
       <c r="A143" s="20" t="s">
         <v>20</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:4" ht="15.75">
       <c r="A144" s="20" t="s">
         <v>20</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:4" ht="15.75">
       <c r="A145" s="20" t="s">
         <v>20</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:4" ht="15.75">
       <c r="A146" s="20" t="s">
         <v>20</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:4" ht="15.75">
       <c r="A147" s="20" t="s">
         <v>20</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:4" ht="15.75">
       <c r="A148" s="20" t="s">
         <v>20</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:4" ht="15.75">
       <c r="A149" s="20" t="s">
         <v>20</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:4" ht="15.75">
       <c r="A150" s="20" t="s">
         <v>20</v>
       </c>
@@ -3947,7 +3947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:4" ht="15.75">
       <c r="A151" s="20" t="s">
         <v>20</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:4" ht="15.75">
       <c r="A152" s="20" t="s">
         <v>20</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:4" ht="15.75">
       <c r="A153" s="20" t="s">
         <v>20</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="154" spans="1:4" ht="16.5" thickBot="1">
       <c r="A154" s="22" t="s">
         <v>20</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:4" ht="15.75">
       <c r="A155" s="20" t="s">
         <v>21</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:4" ht="15.75">
       <c r="A156" s="20" t="s">
         <v>21</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:4" ht="15.75">
       <c r="A157" s="20" t="s">
         <v>21</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:4" ht="15.75">
       <c r="A158" s="20" t="s">
         <v>21</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:4" ht="15.75">
       <c r="A159" s="20" t="s">
         <v>21</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:4" ht="15.75">
       <c r="A160" s="20" t="s">
         <v>21</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:4" ht="15.75">
       <c r="A161" s="20" t="s">
         <v>21</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:4" ht="15.75">
       <c r="A162" s="20" t="s">
         <v>21</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:4" ht="15.75">
       <c r="A163" s="20" t="s">
         <v>21</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:4" ht="15.75">
       <c r="A164" s="20" t="s">
         <v>21</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:4" ht="15.75">
       <c r="A165" s="20" t="s">
         <v>21</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:4" ht="15.75">
       <c r="A166" s="20" t="s">
         <v>21</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:4" ht="15.75">
       <c r="A167" s="20" t="s">
         <v>21</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:4" ht="15.75">
       <c r="A168" s="20" t="s">
         <v>21</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:4" ht="15.75">
       <c r="A169" s="20" t="s">
         <v>21</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:4" ht="15.75">
       <c r="A170" s="20" t="s">
         <v>21</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:4" ht="15.75">
       <c r="A171" s="20" t="s">
         <v>21</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:4" ht="15.75">
       <c r="A172" s="20" t="s">
         <v>21</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:4" ht="15.75">
       <c r="A173" s="20" t="s">
         <v>21</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:4" ht="15.75">
       <c r="A174" s="20" t="s">
         <v>21</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:4" ht="15.75">
       <c r="A175" s="20" t="s">
         <v>21</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:4" ht="15.75">
       <c r="A176" s="20" t="s">
         <v>21</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:4" ht="15.75">
       <c r="A177" s="20" t="s">
         <v>21</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:4" ht="15.75">
       <c r="A178" s="20" t="s">
         <v>21</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="179" spans="1:4" ht="16.5" thickBot="1">
       <c r="A179" s="22" t="s">
         <v>21</v>
       </c>
@@ -4563,28 +4563,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2C79F29-776A-478F-AC44-3E61F39C5C2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2C79F29-776A-478F-AC44-3E61F39C5C2D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F6C018F-5658-4AB1-87EA-C991B973A7AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a26c063d-e4ab-4c2c-a5f9-3b05989843c6"/>
-    <ds:schemaRef ds:uri="31062a0d-ede8-4112-b4bb-00a9c1bc8e16"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F6C018F-5658-4AB1-87EA-C991B973A7AA}"/>
 </file>
</xml_diff>